<commit_message>
Added .ipynb for optical_fiber.4.
</commit_message>
<xml_diff>
--- a/optical_fiber.4/data/data.xlsx
+++ b/optical_fiber.4/data/data.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t xml:space="preserve">mA</t>
   </si>
   <si>
     <t xml:space="preserve">dBm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dBm (cor)</t>
   </si>
   <si>
     <t xml:space="preserve">I = 100 mA</t>
@@ -128,15 +131,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -149,18 +152,35 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -172,16 +192,19 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I1" s="2"/>
     </row>
@@ -192,23 +215,27 @@
       <c r="B2" s="1" t="n">
         <v>-59</v>
       </c>
+      <c r="C2" s="0" t="n">
+        <f aca="false">B2</f>
+        <v>-59</v>
+      </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="I2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -218,23 +245,27 @@
       <c r="B3" s="1" t="n">
         <v>-49</v>
       </c>
+      <c r="C3" s="0" t="n">
+        <f aca="false">B3</f>
+        <v>-49</v>
+      </c>
       <c r="D3" s="1" t="n">
-        <v>0.259</v>
+        <v>0.034</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>9.85</v>
+        <v>3.42</v>
       </c>
       <c r="F3" s="1" t="n">
-        <v>0.107</v>
+        <v>0.035</v>
       </c>
       <c r="G3" s="1" t="n">
-        <v>11.4</v>
+        <v>5.27</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>0.254</v>
+        <v>0.034</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>6.95</v>
+        <v>2.37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -244,23 +275,27 @@
       <c r="B4" s="1" t="n">
         <v>-7.7</v>
       </c>
+      <c r="C4" s="0" t="n">
+        <f aca="false">B4</f>
+        <v>-7.7</v>
+      </c>
       <c r="D4" s="1" t="n">
-        <v>0.2</v>
+        <v>0.04</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>9.58</v>
+        <v>5.26</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>0.1</v>
+        <v>0.04</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>11.34</v>
+        <v>7.08</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>0.22</v>
+        <v>0.035</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>6.83</v>
+        <v>2.65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,23 +305,27 @@
       <c r="B5" s="1" t="n">
         <v>3.45</v>
       </c>
+      <c r="C5" s="0" t="n">
+        <f aca="false">B5</f>
+        <v>3.45</v>
+      </c>
       <c r="D5" s="1" t="n">
-        <v>0.18</v>
+        <v>0.05</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>9.45</v>
+        <v>6.5</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>0.09</v>
+        <v>0.045</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>11</v>
+        <v>8.05</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>0.19</v>
+        <v>0.04</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>6.6</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -296,23 +335,27 @@
       <c r="B6" s="1" t="n">
         <v>5.31</v>
       </c>
+      <c r="C6" s="0" t="n">
+        <f aca="false">B6</f>
+        <v>5.31</v>
+      </c>
       <c r="D6" s="1" t="n">
-        <v>0.23</v>
+        <v>0.06</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>9.75</v>
+        <v>7.25</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>10.64</v>
+        <v>8.7</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>0.17</v>
+        <v>0.045</v>
       </c>
       <c r="I6" s="3" t="n">
-        <v>6.5</v>
+        <v>4.06</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -322,23 +365,27 @@
       <c r="B7" s="1" t="n">
         <v>7.65</v>
       </c>
+      <c r="C7" s="0" t="n">
+        <f aca="false">B7</f>
+        <v>7.65</v>
+      </c>
       <c r="D7" s="1" t="n">
-        <v>0.16</v>
+        <v>0.08</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>9.32</v>
+        <v>8.1</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>0.07</v>
+        <v>0.06</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>10.25</v>
+        <v>9.7</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>6.37</v>
+        <v>4.45</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -348,23 +395,27 @@
       <c r="B8" s="1" t="n">
         <v>9.16</v>
       </c>
+      <c r="C8" s="0" t="n">
+        <f aca="false">B8</f>
+        <v>9.16</v>
+      </c>
       <c r="D8" s="1" t="n">
-        <v>0.14</v>
+        <v>0.1</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>9.14</v>
+        <v>8.53</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>0.06</v>
+        <v>0.07</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>9.7</v>
+        <v>10.25</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>0.12</v>
+        <v>0.054</v>
       </c>
       <c r="I8" s="3" t="n">
-        <v>6.2</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -375,16 +426,16 @@
         <v>8.93</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="G9" s="1" t="n">
-        <v>8.7</v>
+        <v>10.64</v>
       </c>
       <c r="H9" s="3" t="n">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="I9" s="3" t="n">
-        <v>5.97</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -394,23 +445,27 @@
       <c r="B10" s="1" t="n">
         <v>-8.15</v>
       </c>
+      <c r="C10" s="0" t="n">
+        <f aca="false">B10 + ($B$8 - $B$10)</f>
+        <v>9.16</v>
+      </c>
       <c r="D10" s="1" t="n">
-        <v>0.1</v>
+        <v>0.14</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>8.53</v>
+        <v>9.14</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>0.045</v>
+        <v>0.09</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>8.05</v>
+        <v>11</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>0.09</v>
+        <v>0.07</v>
       </c>
       <c r="I10" s="3" t="n">
-        <v>5.8</v>
+        <v>5.38</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -420,17 +475,21 @@
       <c r="B11" s="1" t="n">
         <v>-7.08</v>
       </c>
+      <c r="C11" s="0" t="n">
+        <f aca="false">B11 + ($B$8 - $B$10)</f>
+        <v>10.23</v>
+      </c>
       <c r="D11" s="1" t="n">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>8.1</v>
+        <v>9.32</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>7.08</v>
+        <v>11.34</v>
       </c>
       <c r="H11" s="3" t="n">
         <v>0.08</v>
@@ -446,23 +505,27 @@
       <c r="B12" s="1" t="n">
         <v>-6.24</v>
       </c>
+      <c r="C12" s="0" t="n">
+        <f aca="false">B12 + ($B$8 - $B$10)</f>
+        <v>11.07</v>
+      </c>
       <c r="D12" s="1" t="n">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>7.25</v>
+        <v>9.45</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>0.035</v>
+        <v>0.107</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>5.27</v>
+        <v>11.4</v>
       </c>
       <c r="H12" s="3" t="n">
-        <v>0.07</v>
+        <v>0.09</v>
       </c>
       <c r="I12" s="3" t="n">
-        <v>5.38</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -472,17 +535,21 @@
       <c r="B13" s="1" t="n">
         <v>-5.54</v>
       </c>
+      <c r="C13" s="0" t="n">
+        <f aca="false">B13 + ($B$8 - $B$10)</f>
+        <v>11.77</v>
+      </c>
       <c r="D13" s="1" t="n">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>6.5</v>
+        <v>9.58</v>
       </c>
       <c r="H13" s="3" t="n">
-        <v>0.06</v>
+        <v>0.1</v>
       </c>
       <c r="I13" s="3" t="n">
-        <v>5</v>
+        <v>5.97</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -492,17 +559,21 @@
       <c r="B14" s="1" t="n">
         <v>-4.43</v>
       </c>
+      <c r="C14" s="0" t="n">
+        <f aca="false">B14 + ($B$8 - $B$10)</f>
+        <v>12.88</v>
+      </c>
       <c r="D14" s="1" t="n">
-        <v>0.04</v>
+        <v>0.23</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>5.26</v>
+        <v>9.75</v>
       </c>
       <c r="H14" s="3" t="n">
-        <v>0.054</v>
+        <v>0.12</v>
       </c>
       <c r="I14" s="3" t="n">
-        <v>4.8</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -512,17 +583,21 @@
       <c r="B15" s="1" t="n">
         <v>-3.55</v>
       </c>
+      <c r="C15" s="0" t="n">
+        <f aca="false">B15 + ($B$8 - $B$10)</f>
+        <v>13.76</v>
+      </c>
       <c r="D15" s="1" t="n">
-        <v>0.034</v>
+        <v>0.259</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>3.42</v>
+        <v>9.85</v>
       </c>
       <c r="H15" s="3" t="n">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="I15" s="3" t="n">
-        <v>4.45</v>
+        <v>6.37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -532,11 +607,15 @@
       <c r="B16" s="1" t="n">
         <v>-2.83</v>
       </c>
+      <c r="C16" s="0" t="n">
+        <f aca="false">B16 + ($B$8 - $B$10)</f>
+        <v>14.48</v>
+      </c>
       <c r="H16" s="3" t="n">
-        <v>0.045</v>
+        <v>0.17</v>
       </c>
       <c r="I16" s="3" t="n">
-        <v>4.06</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -546,11 +625,15 @@
       <c r="B17" s="1" t="n">
         <v>-2.23</v>
       </c>
+      <c r="C17" s="0" t="n">
+        <f aca="false">B17 + ($B$8 - $B$10)</f>
+        <v>15.08</v>
+      </c>
       <c r="H17" s="3" t="n">
-        <v>0.04</v>
+        <v>0.19</v>
       </c>
       <c r="I17" s="3" t="n">
-        <v>3.6</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -560,11 +643,15 @@
       <c r="B18" s="1" t="n">
         <v>-1.7</v>
       </c>
+      <c r="C18" s="0" t="n">
+        <f aca="false">B18 + ($B$8 - $B$10)</f>
+        <v>15.61</v>
+      </c>
       <c r="H18" s="3" t="n">
-        <v>0.035</v>
+        <v>0.22</v>
       </c>
       <c r="I18" s="3" t="n">
-        <v>2.65</v>
+        <v>6.83</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -574,11 +661,15 @@
       <c r="B19" s="1" t="n">
         <v>-0.65</v>
       </c>
+      <c r="C19" s="0" t="n">
+        <f aca="false">B19 + ($B$8 - $B$10)</f>
+        <v>16.66</v>
+      </c>
       <c r="H19" s="3" t="n">
-        <v>0.034</v>
+        <v>0.254</v>
       </c>
       <c r="I19" s="3" t="n">
-        <v>2.37</v>
+        <v>6.95</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -588,45 +679,69 @@
       <c r="B20" s="1" t="n">
         <v>0.14</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="n">
+        <f aca="false">B20 + ($B$8 - $B$10)</f>
+        <v>17.45</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>700</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="0" t="n">
+        <f aca="false">B21 + ($B$8 - $B$10)</f>
+        <v>18.11</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>800</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>1.35</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C22" s="0" t="n">
+        <f aca="false">B22 + ($B$8 - $B$10)</f>
+        <v>18.66</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
         <v>900</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="0" t="n">
+        <f aca="false">B23 + ($B$8 - $B$10)</f>
+        <v>19.11</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
         <v>1000</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>2.2</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="0" t="n">
+        <f aca="false">B24 + ($B$8 - $B$10)</f>
+        <v>19.51</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
         <v>1090</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>2.51</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <f aca="false">B25 + ($B$8 - $B$10)</f>
+        <v>19.82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>